<commit_message>
Minor changes to seminar schedule and efrogs
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D987BE6-08D1-45E5-9B15-7846047C9747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1AB9FE-A34B-4666-9E25-9E70D3BB6B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="314">
   <si>
     <t>Date</t>
   </si>
@@ -97,18 +97,9 @@
     <t>Khoa Vu</t>
   </si>
   <si>
-    <t>Vanee Dusoruth</t>
-  </si>
-  <si>
-    <t>Julieth Santamaria</t>
-  </si>
-  <si>
     <t>Alumni, U St. Thomas</t>
   </si>
   <si>
-    <t xml:space="preserve">Alumni </t>
-  </si>
-  <si>
     <t>Webscraping in R and Python</t>
   </si>
   <si>
@@ -730,9 +721,6 @@
     <t>Adriana Castillo Castillo</t>
   </si>
   <si>
-    <t xml:space="preserve">Mwaso </t>
-  </si>
-  <si>
     <t xml:space="preserve">Notes for Job Market Panel: </t>
   </si>
   <si>
@@ -841,18 +829,9 @@
     <t>Soft Skill</t>
   </si>
   <si>
-    <t>dusor001@umn.edu    vaneeshadusoruth@gmail.com</t>
-  </si>
-  <si>
-    <t>a workshop on her experience working at Amazon and what tools or skills does she use in her job (what skills should we be learning)</t>
-  </si>
-  <si>
     <t>Doubly Robust Estimator and Covariate Selection</t>
   </si>
   <si>
-    <t>Alumni in Tech</t>
-  </si>
-  <si>
     <t>Cori Marson</t>
   </si>
   <si>
@@ -865,9 +844,6 @@
     <t>Tips and Tricks with using Linked Census Data</t>
   </si>
   <si>
-    <t xml:space="preserve">shift-share instrument (bartik) </t>
-  </si>
-  <si>
     <t>Abel Broduer</t>
   </si>
   <si>
@@ -955,9 +931,6 @@
     <t>David Redish</t>
   </si>
   <si>
-    <t>Bernard Dalhimer or Raahil Madock</t>
-  </si>
-  <si>
     <t>Experience with government work</t>
   </si>
   <si>
@@ -985,13 +958,28 @@
     <t>Publishing in Interdisciplinary Journals and working with interdiscplinary teams: Perspective from the social sciences and the physical sciences</t>
   </si>
   <si>
-    <t>Purdue, Faculty</t>
-  </si>
-  <si>
     <t>Alumni, Banco de Mexico</t>
   </si>
   <si>
     <t>Jose Casco https://www.josecasco.com/_files/ugd/9d1911_52dfc385ff7846d8902a75c244d9febf.pdf</t>
+  </si>
+  <si>
+    <t>Natalia Ordaz Reynoso</t>
+  </si>
+  <si>
+    <t>Alumni 2021, Meta</t>
+  </si>
+  <si>
+    <t>Working in Tech Sector as an Economist</t>
+  </si>
+  <si>
+    <t>Alumni in Tech (Yufeng Lai https://www.laiyufeng.com/)</t>
+  </si>
+  <si>
+    <t>Raahil Madock</t>
+  </si>
+  <si>
+    <t>Using the Bartik Instrument Variable (Shift-share IV)</t>
   </si>
 </sst>
 </file>
@@ -1464,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D9866-1A44-4963-B386-3AED68110417}">
   <dimension ref="A1:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AE16" sqref="AE16"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1477,7 +1465,7 @@
     <col min="12" max="12" width="18.88671875" customWidth="1"/>
     <col min="13" max="13" width="4.109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="11.88671875" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" style="13" customWidth="1"/>
+    <col min="15" max="15" width="19.77734375" style="13" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.109375" style="13" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.6640625" customWidth="1"/>
     <col min="18" max="18" width="11.88671875" style="12" customWidth="1"/>
@@ -1527,13 +1515,13 @@
       <c r="V1" s="21"/>
       <c r="W1" s="1"/>
       <c r="Y1" s="21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="Z1" s="21"/>
       <c r="AA1" s="21"/>
       <c r="AB1" s="21"/>
       <c r="AD1" s="21" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="AE1" s="21"/>
       <c r="AF1" s="21"/>
@@ -1541,7 +1529,7 @@
       <c r="AH1" s="21"/>
       <c r="AI1" s="21"/>
       <c r="AK1" s="21" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="AL1" s="21"/>
       <c r="AM1" s="21"/>
@@ -1554,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
@@ -1563,7 +1551,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>2</v>
@@ -1590,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>14</v>
@@ -1620,13 +1608,13 @@
         <v>2</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>1</v>
@@ -1655,43 +1643,43 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="4"/>
       <c r="M3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="W3" s="4"/>
       <c r="X3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="AC3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AL3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AO3" s="4" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -1700,514 +1688,521 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="F4" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="G4" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="P4" s="13" t="s">
         <v>15</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="T4" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="W4" s="4"/>
       <c r="X4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y4" s="4"/>
       <c r="AC4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD4" t="s">
         <v>13</v>
       </c>
       <c r="AE4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="AF4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="AH4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="AI4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AL4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP4" s="4" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="4"/>
       <c r="M5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="O5" s="13" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="P5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="S5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="T5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y5" s="4"/>
       <c r="AC5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G6" s="8"/>
       <c r="K6" s="8"/>
       <c r="L6" s="4"/>
       <c r="M6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="O6" s="13" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>15</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="S6" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="T6" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="W6" s="4"/>
       <c r="X6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y6" s="4"/>
       <c r="AC6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD6" t="s">
         <v>13</v>
       </c>
       <c r="AE6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="AI6">
         <v>2024</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AK6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AN6" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP6" s="4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="AQ6" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="4"/>
       <c r="M7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="O7" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>40</v>
       </c>
       <c r="P7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="S7" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="T7" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="W7" s="4"/>
       <c r="X7" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y7" s="4"/>
       <c r="AC7" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD7" t="s">
         <v>13</v>
       </c>
       <c r="AE7" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="AI7">
         <v>2024</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AL7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="AN7" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP7" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="AQ7" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="AR7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="K8" s="8"/>
       <c r="L8" s="4"/>
       <c r="M8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="O8" s="13" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="P8" s="13" t="s">
         <v>15</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="S8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="T8" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="W8" s="4"/>
       <c r="X8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD8" t="s">
         <v>13</v>
       </c>
       <c r="AE8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AI8">
         <v>2024</v>
       </c>
       <c r="AJ8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AL8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="AM8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AN8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP8" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="AQ8" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AR8" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="4"/>
       <c r="M9" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>260</v>
+        <v>256</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="P9" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="Q9" s="13"/>
+      <c r="R9" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="S9" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="T9" s="12" t="s">
+        <v>310</v>
+      </c>
       <c r="W9" s="4"/>
       <c r="X9" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD9" t="s">
         <v>13</v>
       </c>
       <c r="AE9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="AI9">
         <v>2024</v>
       </c>
       <c r="AJ9" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AL9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="AM9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="AN9" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP9" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="AQ9" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AR9" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K10" s="8"/>
       <c r="L10" s="4"/>
       <c r="M10" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="W10" s="4"/>
       <c r="X10" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="Z10" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD10" t="s">
         <v>13</v>
       </c>
       <c r="AE10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="AH10" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="AI10">
         <v>2024</v>
       </c>
       <c r="AJ10" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN10" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP10" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="AQ10" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AR10" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="L11" s="4"/>
       <c r="M11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="P11" t="s">
-        <v>19</v>
+        <v>311</v>
       </c>
       <c r="Q11" t="s">
-        <v>267</v>
+        <v>197</v>
       </c>
       <c r="R11" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="S11" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="W11" s="4"/>
       <c r="X11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y11" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>230</v>
-      </c>
-      <c r="AI11">
-        <v>2024</v>
+        <v>34</v>
       </c>
       <c r="AJ11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP11" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="AQ11" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AR11" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="D12" s="9"/>
       <c r="L12" s="4"/>
       <c r="M12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O12" t="s">
-        <v>63</v>
-      </c>
-      <c r="P12" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>315</v>
-      </c>
-      <c r="R12" t="s">
-        <v>284</v>
-      </c>
-      <c r="S12" t="s">
-        <v>275</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="O12"/>
       <c r="W12" s="4"/>
       <c r="X12" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y12" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>304</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>278</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>305</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP12" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="AQ12" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AR12" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.3">
@@ -2216,7 +2211,7 @@
       <c r="I13" s="9"/>
       <c r="L13" s="4"/>
       <c r="M13" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13"/>
@@ -2225,25 +2220,40 @@
       <c r="T13" s="9"/>
       <c r="W13" s="4"/>
       <c r="X13" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y13" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AC13" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>307</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>306</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>278</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>297</v>
       </c>
       <c r="AJ13" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN13" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP13" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="AQ13" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.3">
@@ -2252,10 +2262,10 @@
       <c r="G14" s="9"/>
       <c r="L14" s="4"/>
       <c r="M14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="O14" s="16"/>
       <c r="P14" s="11"/>
@@ -2264,44 +2274,44 @@
       <c r="S14" s="9"/>
       <c r="W14" s="4"/>
       <c r="X14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Y14" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AA14" s="4"/>
       <c r="AC14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AD14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AE14" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="AF14" t="s">
-        <v>174</v>
+        <v>39</v>
       </c>
       <c r="AG14" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="AH14" t="s">
-        <v>314</v>
+        <v>172</v>
       </c>
       <c r="AJ14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AN14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AP14" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="AQ14" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AR14" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.3">
@@ -2310,67 +2320,67 @@
       <c r="H15" s="8"/>
       <c r="L15" s="4"/>
       <c r="M15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N15" s="8">
         <v>1</v>
       </c>
       <c r="O15" s="16" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>15</v>
       </c>
       <c r="Q15" s="8"/>
       <c r="R15" s="19" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="S15" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="T15" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="W15" s="4"/>
       <c r="X15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y15" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AA15" s="4"/>
       <c r="AC15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD15" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="AE15" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="AF15" t="s">
-        <v>316</v>
+        <v>19</v>
       </c>
       <c r="AG15" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="AH15" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="AJ15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AP15" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="AQ15" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AR15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
@@ -2383,57 +2393,42 @@
       <c r="I16" s="8"/>
       <c r="L16" s="4"/>
       <c r="M16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N16" s="8">
         <v>2</v>
       </c>
       <c r="O16" s="13" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>15</v>
       </c>
       <c r="R16" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="S16" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="T16" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="W16" s="4"/>
       <c r="X16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y16" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="AA16" s="4"/>
       <c r="AC16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE16" t="s">
-        <v>270</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>200</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>283</v>
-      </c>
-      <c r="AH16" t="s">
-        <v>278</v>
+        <v>34</v>
       </c>
       <c r="AJ16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN16" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.3">
@@ -2445,55 +2440,40 @@
       <c r="H17" s="8"/>
       <c r="L17" s="4"/>
       <c r="M17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N17" s="8">
         <v>3</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="P17" s="11"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="W17" s="4"/>
       <c r="X17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y17" s="10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>310</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>284</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>175</v>
+        <v>34</v>
       </c>
       <c r="AJ17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.3">
@@ -2506,31 +2486,57 @@
       <c r="G18" s="9"/>
       <c r="L18" s="4"/>
       <c r="M18" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N18" s="8">
         <v>4</v>
       </c>
-      <c r="O18" s="16"/>
-      <c r="P18" s="11"/>
+      <c r="O18" t="s">
+        <v>312</v>
+      </c>
+      <c r="P18" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="Q18" s="8"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="9"/>
+      <c r="R18" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="S18" t="s">
+        <v>276</v>
+      </c>
+      <c r="T18" t="s">
+        <v>313</v>
+      </c>
       <c r="W18" s="4"/>
       <c r="X18" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y18" s="10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AC18" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>192</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>275</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>20</v>
       </c>
       <c r="AJ18" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN18" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AQ18">
         <f>40/5</f>
@@ -2545,7 +2551,7 @@
       <c r="G19" s="9"/>
       <c r="L19" s="4"/>
       <c r="M19" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N19" s="8">
         <v>5</v>
@@ -2557,34 +2563,34 @@
       <c r="S19" s="9"/>
       <c r="W19" s="4"/>
       <c r="X19" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y19" s="10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="AC19" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AE19" t="s">
-        <v>195</v>
+        <v>61</v>
       </c>
       <c r="AF19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AG19" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="AH19" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="AJ19" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AN19" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.3">
@@ -2596,7 +2602,7 @@
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="M20" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N20" s="8">
         <v>6</v>
@@ -2608,34 +2614,34 @@
       <c r="S20" s="9"/>
       <c r="W20" s="4"/>
       <c r="X20" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Y20" s="10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AC20" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AD20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AE20" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="AF20" t="s">
-        <v>42</v>
+        <v>266</v>
       </c>
       <c r="AG20" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="AH20" t="s">
-        <v>65</v>
+        <v>267</v>
       </c>
       <c r="AJ20" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="AN20" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.3">
@@ -2647,42 +2653,42 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="M21" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="N21" s="8">
         <v>7</v>
       </c>
       <c r="W21" s="4"/>
       <c r="X21" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="Y21" s="10" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="AC21" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AD21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AE21" t="s">
-        <v>54</v>
+        <v>224</v>
       </c>
       <c r="AF21" t="s">
-        <v>273</v>
+        <v>39</v>
       </c>
       <c r="AG21" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="AH21" t="s">
-        <v>274</v>
+        <v>178</v>
       </c>
       <c r="AJ21" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AL21" s="7"/>
       <c r="AN21" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.3">
@@ -2695,295 +2701,256 @@
       <c r="G22" s="9"/>
       <c r="W22" s="4"/>
       <c r="Y22" s="10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AD22" t="s">
-        <v>63</v>
+        <v>221</v>
       </c>
       <c r="AE22" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="AF22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AG22" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="AH22" t="s">
-        <v>181</v>
+        <v>239</v>
       </c>
       <c r="AL22" s="7"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B23" s="17"/>
       <c r="M23" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="W23" s="4"/>
       <c r="X23" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD23" t="s">
-        <v>224</v>
-      </c>
-      <c r="AE23" t="s">
-        <v>225</v>
-      </c>
-      <c r="AF23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AG23" t="s">
-        <v>286</v>
-      </c>
-      <c r="AH23" t="s">
-        <v>243</v>
+        <v>34</v>
       </c>
       <c r="AJ23" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AK23" s="7"/>
       <c r="AL23" s="7"/>
       <c r="AM23" s="7"/>
       <c r="AN23" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M24" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="W24" s="4"/>
       <c r="X24" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AC24" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AJ24" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="AK24" s="7"/>
       <c r="AL24" s="7"/>
       <c r="AN24" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M25" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="W25" s="4"/>
-      <c r="AD25" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>307</v>
-      </c>
-      <c r="AF25" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG25" t="s">
-        <v>286</v>
-      </c>
-      <c r="AH25" t="s">
-        <v>308</v>
-      </c>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE26" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF26" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M27" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M28" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M29" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M30" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M31" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M32" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M33" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M34" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M35" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M36" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M37" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M38" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M39" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M40" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M41" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M42" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M43" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M44" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M45" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M46" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M47" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M48" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M49" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M50" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M51" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M52" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M53" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M54" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M55" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M56" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M57" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M58" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M59" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M60" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M61" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M62" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3004,8 +2971,8 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3018,77 +2985,77 @@
   <sheetData>
     <row r="1" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>15</v>
@@ -3096,10 +3063,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F7" s="13">
         <v>2022</v>
@@ -3107,18 +3074,18 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F9" s="13">
         <v>2022</v>
@@ -3126,37 +3093,37 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C10" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C12" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -3164,31 +3131,31 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>15</v>
@@ -3196,10 +3163,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F18" s="13">
         <v>2020</v>
@@ -3207,37 +3174,37 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D19" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F22" s="13">
         <v>2023</v>
@@ -3248,7 +3215,7 @@
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F23" s="13">
         <v>2023</v>
@@ -3256,26 +3223,26 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -3283,21 +3250,21 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D28" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>15</v>
@@ -3305,26 +3272,26 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F31" s="13">
         <v>2021</v>
@@ -3332,72 +3299,72 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D32" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C35" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D35" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C38" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>15</v>
@@ -3405,21 +3372,21 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F41" s="13">
         <v>2021</v>
@@ -3427,18 +3394,18 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C42" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B43" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F43" s="13">
         <v>2017</v>
@@ -3446,34 +3413,34 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E44" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E45" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E46" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3504,476 +3471,476 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
         <v>81</v>
       </c>
-      <c r="D5" t="s">
-        <v>84</v>
-      </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E28" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E31" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E32" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E33" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E34" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated website for Fall 2024 release
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1AB9FE-A34B-4666-9E25-9E70D3BB6B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8491E43-B085-4DCC-9173-BACD6E84CC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Presentations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="354">
   <si>
     <t>Date</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Advances in RDD methods</t>
   </si>
   <si>
-    <t>Hosam suggested Ozier (2016) on data-driven cutoff detection</t>
-  </si>
-  <si>
     <t>Machine learning applications in economics</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
     <t>Alumni</t>
   </si>
   <si>
-    <t>Fall 2024</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -631,9 +625,6 @@
     <t>MS THESIS SYMPOSIUM</t>
   </si>
   <si>
-    <t>Public Policy PhD Student</t>
-  </si>
-  <si>
     <t>Rebecca Weir</t>
   </si>
   <si>
@@ -715,9 +706,6 @@
     <t>Ryan McWay?</t>
   </si>
   <si>
-    <t>Sarah Walby</t>
-  </si>
-  <si>
     <t>Adriana Castillo Castillo</t>
   </si>
   <si>
@@ -847,12 +835,6 @@
     <t>Abel Broduer</t>
   </si>
   <si>
-    <t xml:space="preserve">      </t>
-  </si>
-  <si>
-    <t>Creating Dashboards for Economics</t>
-  </si>
-  <si>
     <t>Spring Lined Up</t>
   </si>
   <si>
@@ -973,20 +955,158 @@
     <t>Working in Tech Sector as an Economist</t>
   </si>
   <si>
-    <t>Alumni in Tech (Yufeng Lai https://www.laiyufeng.com/)</t>
-  </si>
-  <si>
     <t>Raahil Madock</t>
   </si>
   <si>
     <t>Using the Bartik Instrument Variable (Shift-share IV)</t>
+  </si>
+  <si>
+    <t>Yufeng Lai</t>
+  </si>
+  <si>
+    <t>Alumni 2021, Amazon</t>
+  </si>
+  <si>
+    <t>Non-traditional skills for Economists to Deliver in the Tech Sector</t>
+  </si>
+  <si>
+    <t>Next Semester:</t>
+  </si>
+  <si>
+    <t>Manlin Cui</t>
+  </si>
+  <si>
+    <t>Jiuchen Deng</t>
+  </si>
+  <si>
+    <t>Divya Pandey</t>
+  </si>
+  <si>
+    <t>Qingyin Cai</t>
+  </si>
+  <si>
+    <t>Ana Melissa Perez</t>
+  </si>
+  <si>
+    <t>JMC</t>
+  </si>
+  <si>
+    <t>Payments for Ecosystem Services, Reforestation and Rural Livelihoods</t>
+  </si>
+  <si>
+    <t>Environment, Development</t>
+  </si>
+  <si>
+    <t>Reforestation is crucial for environmental preservation, combating climate change, curbing desertification, and supporting local economies. The Payments for Ecosystem Services (PES) scheme has emerged as a significant policy tool aimed at mitigating deforestation and promoting reforestation. However, the long-term effects of PES schemes on rural livelihoods are under-documented. This study investigates the interaction between environmental goals and distributional outcomes in China's Grain for Green' (GfG) program, one of the world's largest PES programs. Using data from the China's National Rural Fixed Point (NRFP) Survey, we analyze the impact of the GfG program on rural household income, expenditure, and labor allocation. Employing a Difference-in-Differences model, our findings indicate that participation in the GfG program significantly increases household and net household incomes, as well as household and food expenditures. Conversely, the program leads to a decrease in non-farm income and working days, suggesting a shift away from non-farm activities. These results highlight the benefits of the GfG program, promoting both environmental and economic sustainability. Our study contributes valuable insights into the long-term impacts of the GfG program, offering guidance for future PES program implementations and policy designs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ian Luby, lubyx023@umn.edu </t>
+  </si>
+  <si>
+    <t>ABD</t>
+  </si>
+  <si>
+    <t>Mass shootings and their effects on food shopping behavior</t>
+  </si>
+  <si>
+    <t>During the last decade, mass shootings have become the center of attention due to the mental health effects they have on victims. Given the importance of understanding other possible impacts, they may have on the population, not only on the direct victims but on those indirectly affected, this paper aims to understand the potential effects of mass shootings on consumer behavior in affected areas by analyzing changes in the purchase of food items such as sugary drinks, caffeine, and processed foods. Additionally, I examine the impact of mass shootings on the purchase of alcoholic beverages, cigarettes, and painkillers</t>
+  </si>
+  <si>
+    <t>Crime, Health</t>
+  </si>
+  <si>
+    <t>Drought and the Specialty Crop Production in California</t>
+  </si>
+  <si>
+    <t>Environment, Agriculture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California, which supplies a majority of specialty crops in the U.S., has been suffering severe droughts in recent decades. Using county-level panel data, we estimate the impacts of drought, as defined by the U.S. Drought Monitor (USDM), on specialty crop total outputs during the 2000–2019 period. We find the total outputs of specialty crops exhibit a significant negative response to droughts, ranging from -1.2% to -2.2% for an additional week of drought. This reduction in total outputs is attributed to the combined effects of declining yields per acre and harvested acreages under drought conditions. Evidence of response heterogeneity suggests that water-intensive crops and crops with low returns are most affected. These results highlight the importance of enhancing drought-related risk management and provide implications for designing cost-effective policies for future adaptation decisions. </t>
+  </si>
+  <si>
+    <t>The Development of Personality Traits and Cognitive Skills in Adolescence: Evidence from a Skill Formation Model and a Control Function Approach</t>
+  </si>
+  <si>
+    <t>Despite its great importance in child development, education, intra-household allocation, and labor market outcomes, the formation of personality traits remain understudied. I use a skill formation model and a control function approach to investigate the formation of the Big Five personality traits and cognitive skills in adolescence. I find evidence of cross-effects between  personality traits and cognitive skills, which are cross-validated by the findings in neuroscience research. I find strong self-productivity of personality traits and cognitive skills. Based on the control function approach, I uncover a negative impact of maternal hours worked and a positive offsetting effect of family income on adolescents' personality traits and cognitive skills. Results from the skill formation model and the control function approach are consistent internally and with other studies.</t>
+  </si>
+  <si>
+    <t>Behavior, Education</t>
+  </si>
+  <si>
+    <t>Agricultural mechanization and structural transformation</t>
+  </si>
+  <si>
+    <t>Agriculture, Labor, Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Impact of Weather Shocks on Fertility in Rural India</t>
+  </si>
+  <si>
+    <t>Gender, Environment</t>
+  </si>
+  <si>
+    <t>Ivan Strahof</t>
+  </si>
+  <si>
+    <t>ling, monique, econ JMC, policy JMC</t>
+  </si>
+  <si>
+    <t>Sarah Wabhy?</t>
+  </si>
+  <si>
+    <t>Monique Davis?</t>
+  </si>
+  <si>
+    <t>The total fertility rate (TFR) in rural India has fallen by half in recent decades. This paper seeks to understand the role of negative weather shocks in decreasing fertility rates in rural India. I find that the average probability of birth to a woman shows a significant decline in the years following a drought, suggesting adjustment in fertility rates by households following a weather-led adverse economic shock. I also find suggestive evidence that households in drought-prone areas have a preference for significantly smaller family sizes.</t>
+  </si>
+  <si>
+    <t>Evan Cunningham</t>
+  </si>
+  <si>
+    <t>Econ JMC</t>
+  </si>
+  <si>
+    <t>Local Labor Market Effects of Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the arrival of a new, highly productive employer to a local labor market increase welfare for resident workers? To answer this question, I analyze the local labor market effects of the dramatic expansion in Amazon's fulfillment center (FC) network from 2010 onward. I exploit the staggered roll-out of FCs across large U.S. metros in a difference-in-differences framework. After Amazon first expands into a metro, the overall employment rate is 1.0 percentage points higher, average wages increase by 0.7 percent, and the composition of employment shifts from retail and wholesale trade to warehousing and tradable services. Employment gains are concentrated among non-college workers, while younger workers reallocate across sectors more and have higher wage growth. Rents increase by 1.3 percent, utility costs increase by 5.1 percent, and home values in the metro increase by 5.6 percent. I interpret these results through the lens of a spatial equilibrium model. I find the average worker would be willing to pay $349 per year (0.8 percent of after-tax income) to live in a market with Amazon. The incidence varies by home ownership status and education. For renters, the benefits of the positive labor market effects are completely offset by the rising prices; welfare effects are slightly negative. The gains from Amazon's expansion accrue to homeowners via rising home values. Non-college workers also captured larger welfare gains than college-educated and younger workers. </t>
+  </si>
+  <si>
+    <t>Labor, Urban</t>
+  </si>
+  <si>
+    <t>Does agricultural mechanization promote structural transformation, especially in labor-abundant countries? This paper measures the effect of subsidized agricultural mechanization on employment. Using a unique machinery subsidy and purchase dataset, I construct local exposure to a common subsidy policy as a shift-share instrument for mechanization. Two-stage least squares with fixed effects estimates show that mechanization increases employment in the wholesale and retail sectors in the local area and in the manufacturing sector in the migration destinations but has no significant effect on the overall non-agricultural employment. This is confirmed by individual-level analysis, which further reveals that mechanization brings men back to agriculture while leading women to withdraw from both agricultural and non-agricultural jobs. This study shows that mechanization plays a limited role in accelerating structural transformation. In the meantime, it reinforces gender inequality in agriculture.</t>
+  </si>
+  <si>
+    <t>Bixuan Sun</t>
+  </si>
+  <si>
+    <t>Spring 2025</t>
+  </si>
+  <si>
+    <t>PhD student?</t>
+  </si>
+  <si>
+    <t>Kyuseon (Kristy) Lee</t>
+  </si>
+  <si>
+    <t>Steve Miller</t>
+  </si>
+  <si>
+    <t>Past Faculty</t>
+  </si>
+  <si>
+    <t>Faculty, Alumni 2015</t>
+  </si>
+  <si>
+    <t>Yes?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1040,6 +1160,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1088,7 +1215,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1132,6 +1259,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1452,16 +1583,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D9866-1A44-4963-B386-3AED68110417}">
   <dimension ref="A1:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="11" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="11" width="11.6640625" customWidth="1"/>
     <col min="12" max="12" width="18.88671875" customWidth="1"/>
     <col min="13" max="13" width="4.109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="11.88671875" customWidth="1"/>
@@ -1488,51 +1622,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
       <c r="L1" s="1"/>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
       <c r="W1" s="1"/>
-      <c r="Y1" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AD1" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
-      <c r="AK1" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
+      <c r="Y1" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AD1" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AK1" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1541,17 +1675,17 @@
       <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>2</v>
@@ -1578,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>14</v>
@@ -1608,13 +1742,13 @@
         <v>2</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="AE2" s="2" t="s">
         <v>1</v>
@@ -1643,338 +1777,523 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="K3" s="8"/>
+        <v>239</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="G3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H3" t="s">
+        <v>345</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>63</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>244</v>
+        <v>240</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="T3" t="s">
+        <v>309</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="W3" s="4"/>
       <c r="X3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y3" s="4"/>
       <c r="AC3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>347</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AL3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AN3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AO3" s="4" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>294</v>
+        <v>177</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>288</v>
       </c>
       <c r="F4" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G4" t="s">
-        <v>293</v>
+        <v>287</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="P4" s="13" t="s">
         <v>15</v>
       </c>
+      <c r="Q4" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="R4" s="12" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="S4" s="13" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="T4" t="s">
-        <v>303</v>
+        <v>297</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="W4" s="4"/>
       <c r="X4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y4" s="4"/>
       <c r="AC4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD4" t="s">
         <v>13</v>
       </c>
       <c r="AE4" t="s">
+        <v>346</v>
+      </c>
+      <c r="AF4" t="s">
         <v>65</v>
       </c>
-      <c r="AF4" t="s">
-        <v>66</v>
-      </c>
       <c r="AH4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AI4" t="s">
-        <v>67</v>
+        <v>347</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AL4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AN4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP4" s="4" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="K5" s="8"/>
+        <v>243</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>184</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="M5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="O5" s="13" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="P5" s="13" t="s">
         <v>15</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="S5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T5" t="s">
-        <v>259</v>
+        <v>255</v>
+      </c>
+      <c r="U5" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y5" s="4"/>
       <c r="AC5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>222</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>347</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AN5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="G6" s="8"/>
+        <v>245</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="G6" t="s">
+        <v>342</v>
+      </c>
+      <c r="H6" t="s">
+        <v>343</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>15</v>
+      </c>
       <c r="K6" s="8"/>
       <c r="L6" s="4"/>
       <c r="M6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="O6" s="13" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>15</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>171</v>
+        <v>352</v>
       </c>
       <c r="S6" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="T6" t="s">
-        <v>273</v>
+        <v>267</v>
+      </c>
+      <c r="U6" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="W6" s="4"/>
       <c r="X6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y6" s="4"/>
       <c r="AC6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD6" t="s">
         <v>13</v>
       </c>
       <c r="AE6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI6">
-        <v>2024</v>
+        <v>349</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>347</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AK6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="AN6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP6" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AQ6" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="K7" s="8"/>
+        <v>247</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="G7" t="s">
+        <v>333</v>
+      </c>
+      <c r="H7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>311</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="O7" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="R7" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S7" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="T7" t="s">
-        <v>263</v>
+        <v>259</v>
+      </c>
+      <c r="U7" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="W7" s="4"/>
       <c r="X7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y7" s="4"/>
       <c r="AC7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD7" t="s">
         <v>13</v>
       </c>
       <c r="AE7" t="s">
-        <v>192</v>
-      </c>
-      <c r="AI7">
-        <v>2024</v>
+        <v>320</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>347</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AL7" t="s">
         <v>22</v>
       </c>
       <c r="AN7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP7" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="AQ7" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="AR7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="K8" s="8"/>
+        <v>249</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>326</v>
+      </c>
+      <c r="G8" t="s">
+        <v>325</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>327</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>195</v>
+      </c>
       <c r="L8" s="4"/>
       <c r="M8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="O8" s="13" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="P8" s="13" t="s">
         <v>15</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="S8" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="T8" t="s">
-        <v>291</v>
+        <v>285</v>
+      </c>
+      <c r="U8" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="W8" s="4"/>
       <c r="X8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>198</v>
-      </c>
-      <c r="AI8">
-        <v>2024</v>
+        <v>33</v>
       </c>
       <c r="AJ8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AL8" t="s">
         <v>23</v>
@@ -1983,235 +2302,293 @@
         <v>21</v>
       </c>
       <c r="AN8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP8" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="AQ8" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AR8" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>255</v>
+        <v>251</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" t="s">
+        <v>318</v>
+      </c>
+      <c r="G9" t="s">
+        <v>317</v>
+      </c>
+      <c r="H9" t="s">
+        <v>319</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="K9" s="8"/>
       <c r="L9" s="4"/>
       <c r="M9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="O9" s="13" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="P9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Q9" s="13"/>
+      <c r="Q9" s="13" t="s">
+        <v>353</v>
+      </c>
       <c r="R9" s="12" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="S9" s="13" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="T9" s="12" t="s">
-        <v>310</v>
+        <v>304</v>
+      </c>
+      <c r="U9" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="W9" s="4"/>
       <c r="X9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD9" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="AE9" t="s">
-        <v>226</v>
-      </c>
-      <c r="AI9">
-        <v>2024</v>
+        <v>301</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>300</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>272</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>291</v>
       </c>
       <c r="AJ9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL9" t="s">
-        <v>25</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="AN9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP9" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="AQ9" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AR9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="K10" s="8"/>
+        <v>253</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>335</v>
+      </c>
       <c r="L10" s="4"/>
       <c r="M10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W10" s="4"/>
       <c r="X10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Z10" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD10" t="s">
         <v>13</v>
       </c>
       <c r="AE10" t="s">
-        <v>225</v>
+        <v>292</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>272</v>
       </c>
       <c r="AH10" t="s">
-        <v>269</v>
-      </c>
-      <c r="AI10">
-        <v>2024</v>
+        <v>293</v>
       </c>
       <c r="AJ10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AN10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP10" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="AQ10" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AR10" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="L11" s="4"/>
       <c r="M11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O11" t="s">
-        <v>60</v>
-      </c>
-      <c r="P11" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>197</v>
-      </c>
-      <c r="R11" t="s">
-        <v>275</v>
-      </c>
-      <c r="S11" t="s">
-        <v>270</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="R11"/>
       <c r="W11" s="4"/>
       <c r="X11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>295</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>270</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>170</v>
       </c>
       <c r="AJ11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP11" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="AQ11" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AR11" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="D12" s="9"/>
+      <c r="D12" s="21"/>
       <c r="L12" s="4"/>
       <c r="M12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O12"/>
       <c r="W12" s="4"/>
       <c r="X12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y12" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE12" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="AF12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="AG12" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="AH12" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP12" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="AQ12" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AR12" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
       <c r="I13" s="9"/>
       <c r="L13" s="4"/>
       <c r="M13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N13" s="9"/>
       <c r="O13"/>
@@ -2220,52 +2597,55 @@
       <c r="T13" s="9"/>
       <c r="W13" s="4"/>
       <c r="X13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y13" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AC13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE13" t="s">
-        <v>307</v>
+        <v>350</v>
       </c>
       <c r="AF13" t="s">
-        <v>306</v>
+        <v>351</v>
       </c>
       <c r="AG13" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="AH13" t="s">
-        <v>297</v>
+        <v>24</v>
       </c>
       <c r="AJ13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AN13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AP13" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AQ13" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>195</v>
+      </c>
       <c r="C14" s="11"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="1"/>
       <c r="G14" s="9"/>
       <c r="L14" s="4"/>
       <c r="M14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="O14" s="16"/>
       <c r="P14" s="11"/>
@@ -2274,118 +2654,109 @@
       <c r="S14" s="9"/>
       <c r="W14" s="4"/>
       <c r="X14" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y14" s="10" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AA14" s="4"/>
       <c r="AC14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>301</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG14" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>281</v>
+      </c>
+      <c r="AQ14" t="s">
         <v>276</v>
       </c>
-      <c r="AH14" t="s">
-        <v>172</v>
-      </c>
-      <c r="AJ14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP14" t="s">
-        <v>287</v>
-      </c>
-      <c r="AQ14" t="s">
-        <v>282</v>
-      </c>
       <c r="AR14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="B15" s="13" t="s">
+        <v>311</v>
+      </c>
       <c r="C15" s="11"/>
       <c r="G15" s="9"/>
       <c r="H15" s="8"/>
       <c r="L15" s="4"/>
       <c r="M15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N15" s="8">
         <v>1</v>
       </c>
       <c r="O15" s="16" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>15</v>
       </c>
       <c r="Q15" s="8"/>
       <c r="R15" s="19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="S15" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="T15" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="W15" s="4"/>
       <c r="X15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y15" s="10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AA15" s="4"/>
       <c r="AC15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD15" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="AE15" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="AF15" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="AG15" t="s">
+        <v>269</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>20</v>
+      </c>
+      <c r="AJ15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AN15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP15" t="s">
         <v>278</v>
       </c>
-      <c r="AH15" t="s">
-        <v>299</v>
-      </c>
-      <c r="AJ15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AN15" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AP15" t="s">
-        <v>284</v>
-      </c>
       <c r="AQ15" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AR15" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>337</v>
+      </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="8"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -2393,150 +2764,185 @@
       <c r="I16" s="8"/>
       <c r="L16" s="4"/>
       <c r="M16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N16" s="8">
         <v>2</v>
       </c>
       <c r="O16" s="13" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>15</v>
       </c>
       <c r="R16" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S16" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="T16" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="W16" s="4"/>
       <c r="X16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y16" s="10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="AA16" s="4"/>
       <c r="AC16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>272</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>61</v>
       </c>
       <c r="AJ16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AN16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C17" s="11"/>
-      <c r="D17" s="8"/>
+      <c r="B17" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="8"/>
       <c r="L17" s="4"/>
       <c r="M17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N17" s="8">
         <v>3</v>
       </c>
       <c r="O17" s="16" t="s">
-        <v>289</v>
-      </c>
-      <c r="P17" s="11"/>
+        <v>283</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>336</v>
+      </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S17" s="8" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="T17" s="8" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="W17" s="4"/>
       <c r="X17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y17" s="10" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AC17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>262</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>269</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>263</v>
       </c>
       <c r="AJ17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AN17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="16"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="8"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="L18" s="4"/>
       <c r="M18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N18" s="8">
         <v>4</v>
       </c>
-      <c r="O18" t="s">
-        <v>312</v>
+      <c r="O18" s="13" t="s">
+        <v>305</v>
       </c>
       <c r="P18" s="11" t="s">
         <v>15</v>
       </c>
       <c r="Q18" s="8"/>
-      <c r="R18" s="20" t="s">
-        <v>171</v>
+      <c r="R18" s="19" t="s">
+        <v>169</v>
       </c>
       <c r="S18" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="T18" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="W18" s="4"/>
       <c r="X18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y18" s="10" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AC18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE18" t="s">
-        <v>192</v>
+        <v>221</v>
       </c>
       <c r="AF18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG18" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="AH18" t="s">
-        <v>20</v>
+        <v>176</v>
       </c>
       <c r="AJ18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AN18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AQ18">
         <f>40/5</f>
@@ -2551,7 +2957,7 @@
       <c r="G19" s="9"/>
       <c r="L19" s="4"/>
       <c r="M19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N19" s="8">
         <v>5</v>
@@ -2563,46 +2969,46 @@
       <c r="S19" s="9"/>
       <c r="W19" s="4"/>
       <c r="X19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y19" s="10" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="AC19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD19" t="s">
-        <v>60</v>
+        <v>218</v>
       </c>
       <c r="AE19" t="s">
-        <v>61</v>
+        <v>219</v>
       </c>
       <c r="AF19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG19" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="AH19" t="s">
-        <v>62</v>
+        <v>235</v>
       </c>
       <c r="AJ19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AN19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="16"/>
       <c r="C20" s="11"/>
-      <c r="D20" s="8"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="M20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N20" s="8">
         <v>6</v>
@@ -2614,343 +3020,299 @@
       <c r="S20" s="9"/>
       <c r="W20" s="4"/>
       <c r="X20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y20" s="10" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="AC20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD20" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE20" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>266</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>275</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>267</v>
+        <v>34</v>
       </c>
       <c r="AJ20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AN20" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="16"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="8"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="M21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N21" s="8">
         <v>7</v>
       </c>
       <c r="W21" s="4"/>
       <c r="X21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y21" s="10" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AC21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD21" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE21" t="s">
-        <v>224</v>
-      </c>
-      <c r="AF21" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG21" t="s">
-        <v>276</v>
-      </c>
-      <c r="AH21" t="s">
-        <v>178</v>
+        <v>33</v>
       </c>
       <c r="AJ21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AL21" s="7"/>
       <c r="AN21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="16"/>
       <c r="C22" s="11"/>
-      <c r="D22" s="8"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="W22" s="4"/>
       <c r="Y22" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="AD22" t="s">
-        <v>221</v>
-      </c>
-      <c r="AE22" t="s">
-        <v>222</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>278</v>
-      </c>
-      <c r="AH22" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="AL22" s="7"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
       <c r="M23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W23" s="4"/>
       <c r="X23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AJ23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AK23" s="7"/>
       <c r="AL23" s="7"/>
       <c r="AM23" s="7"/>
       <c r="AN23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="D24" s="1"/>
       <c r="M24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W24" s="4"/>
       <c r="X24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AJ24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AK24" s="7"/>
       <c r="AL24" s="7"/>
       <c r="AN24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W25" s="4"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.3">
       <c r="M32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M34" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M38" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M39" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M40" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M41" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M43" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M44" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M45" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M46" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M47" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M48" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M49" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M50" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M51" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M52" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M53" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M54" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M55" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M56" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M57" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M58" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M59" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M60" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M61" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M62" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2985,77 +3347,77 @@
   <sheetData>
     <row r="1" spans="1:8" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>15</v>
@@ -3063,10 +3425,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
         <v>52</v>
-      </c>
-      <c r="B7" t="s">
-        <v>53</v>
       </c>
       <c r="F7" s="13">
         <v>2022</v>
@@ -3074,18 +3436,18 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="13">
         <v>2022</v>
@@ -3093,37 +3455,37 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -3131,31 +3493,31 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D17" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>15</v>
@@ -3163,10 +3525,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="13">
         <v>2020</v>
@@ -3174,37 +3536,37 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D19" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C20" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B22" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F22" s="13">
         <v>2023</v>
@@ -3215,7 +3577,7 @@
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F23" s="13">
         <v>2023</v>
@@ -3223,26 +3585,26 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -3250,21 +3612,21 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D28" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>15</v>
@@ -3272,26 +3634,26 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B30" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" s="13">
         <v>2021</v>
@@ -3299,72 +3661,72 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D32" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" t="s">
         <v>43</v>
-      </c>
-      <c r="B34" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C35" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D35" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B36" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C38" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>15</v>
@@ -3372,21 +3734,21 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F41" s="13">
         <v>2021</v>
@@ -3394,18 +3756,18 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C42" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B43" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F43" s="13">
         <v>2017</v>
@@ -3413,34 +3775,34 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E44" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E45" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E46" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E47" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3471,476 +3833,476 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
         <v>78</v>
       </c>
-      <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="s">
-        <v>80</v>
-      </c>
       <c r="F5" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>143</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
         <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" t="s">
         <v>102</v>
-      </c>
-      <c r="D15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="D19" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="D21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" t="s">
         <v>105</v>
       </c>
-      <c r="D22" t="s">
-        <v>107</v>
-      </c>
       <c r="E22" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" t="s">
         <v>99</v>
-      </c>
-      <c r="D23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" t="s">
         <v>82</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to notes and attendance log
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8491E43-B085-4DCC-9173-BACD6E84CC23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF85B1A-7C01-4570-98D4-8606BCB88131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="354">
   <si>
     <t>Date</t>
   </si>
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D9866-1A44-4963-B386-3AED68110417}">
   <dimension ref="A1:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2339,7 +2339,9 @@
       <c r="I9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>154</v>
+      </c>
       <c r="L9" s="4"/>
       <c r="M9" s="3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Attendance update and women in APEC material
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF85B1A-7C01-4570-98D4-8606BCB88131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C89F8B-9271-4B40-A6B5-194A5F9C9D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Presentations" sheetId="1" r:id="rId1"/>
@@ -1583,8 +1583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D9866-1A44-4963-B386-3AED68110417}">
   <dimension ref="A1:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Started scheduling for Spring 2025 in notes
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C89F8B-9271-4B40-A6B5-194A5F9C9D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49512439-A6C6-4736-973C-539D6139E3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Presentations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="359">
   <si>
     <t>Date</t>
   </si>
@@ -1048,15 +1048,6 @@
     <t>Ivan Strahof</t>
   </si>
   <si>
-    <t>ling, monique, econ JMC, policy JMC</t>
-  </si>
-  <si>
-    <t>Sarah Wabhy?</t>
-  </si>
-  <si>
-    <t>Monique Davis?</t>
-  </si>
-  <si>
     <t>The total fertility rate (TFR) in rural India has fallen by half in recent decades. This paper seeks to understand the role of negative weather shocks in decreasing fertility rates in rural India. I find that the average probability of birth to a woman shows a significant decline in the years following a drought, suggesting adjustment in fertility rates by households following a weather-led adverse economic shock. I also find suggestive evidence that households in drought-prone areas have a preference for significantly smaller family sizes.</t>
   </si>
   <si>
@@ -1100,12 +1091,39 @@
   </si>
   <si>
     <t>Yes?</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>SPRING BREAK</t>
+  </si>
+  <si>
+    <t>workshop</t>
+  </si>
+  <si>
+    <t>Schedule the 4 speaker slots, and then remove remaining workshops</t>
+  </si>
+  <si>
+    <t>Send call for presenters, all options, then select a couple for free discussions</t>
+  </si>
+  <si>
+    <t>Then settle on schedule and annonce</t>
+  </si>
+  <si>
+    <t>Wednesdays from 11 AM - 12 PM</t>
+  </si>
+  <si>
+    <t>ling, monique, econ JMC,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1215,7 +1233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1266,6 +1284,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1584,12 +1603,12 @@
   <dimension ref="A1:AR62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" style="13" customWidth="1"/>
     <col min="3" max="3" width="11.109375" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="13" customWidth="1"/>
@@ -1795,7 +1814,7 @@
         <v>331</v>
       </c>
       <c r="H3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>15</v>
@@ -1849,7 +1868,7 @@
         <v>166</v>
       </c>
       <c r="AI3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AJ3" s="3" t="s">
         <v>33</v>
@@ -1932,7 +1951,7 @@
         <v>13</v>
       </c>
       <c r="AE4" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="AF4" t="s">
         <v>65</v>
@@ -1941,7 +1960,7 @@
         <v>166</v>
       </c>
       <c r="AI4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AJ4" s="3" t="s">
         <v>33</v>
@@ -2035,7 +2054,7 @@
         <v>166</v>
       </c>
       <c r="AI5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AJ5" s="3" t="s">
         <v>33</v>
@@ -2052,22 +2071,22 @@
         <v>245</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="G6" t="s">
+        <v>339</v>
+      </c>
+      <c r="H6" t="s">
         <v>340</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>341</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="G6" t="s">
-        <v>342</v>
-      </c>
-      <c r="H6" t="s">
-        <v>343</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>15</v>
@@ -2087,7 +2106,7 @@
         <v>15</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="S6" t="s">
         <v>269</v>
@@ -2110,7 +2129,7 @@
         <v>13</v>
       </c>
       <c r="AE6" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="AF6" t="s">
         <v>65</v>
@@ -2119,7 +2138,7 @@
         <v>166</v>
       </c>
       <c r="AI6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AJ6" s="3" t="s">
         <v>33</v>
@@ -2157,7 +2176,7 @@
         <v>333</v>
       </c>
       <c r="H7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>15</v>
@@ -2211,7 +2230,7 @@
         <v>166</v>
       </c>
       <c r="AI7" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AJ7" s="3" t="s">
         <v>33</v>
@@ -2356,7 +2375,7 @@
         <v>15</v>
       </c>
       <c r="Q9" s="13" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="R9" s="12" t="s">
         <v>303</v>
@@ -2611,10 +2630,10 @@
         <v>59</v>
       </c>
       <c r="AE13" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="AF13" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="AG13" t="s">
         <v>269</v>
@@ -2726,7 +2745,7 @@
         <v>59</v>
       </c>
       <c r="AE15" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="AF15" t="s">
         <v>38</v>
@@ -2754,9 +2773,6 @@
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
-        <v>337</v>
-      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
@@ -2820,9 +2836,6 @@
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="B17" s="13" t="s">
-        <v>338</v>
-      </c>
       <c r="C17" s="22"/>
       <c r="D17" s="11"/>
       <c r="E17" s="9"/>
@@ -2840,7 +2853,7 @@
         <v>283</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>336</v>
+        <v>358</v>
       </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="19" t="s">
@@ -2964,7 +2977,7 @@
       <c r="N19" s="8">
         <v>5</v>
       </c>
-      <c r="O19" s="16"/>
+      <c r="O19"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="20"/>
@@ -3002,10 +3015,16 @@
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="24">
+        <v>45679</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>351</v>
+      </c>
       <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
+      <c r="D20" s="12" t="s">
+        <v>357</v>
+      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -3038,10 +3057,16 @@
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="24">
+        <v>45686</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>353</v>
+      </c>
       <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
+      <c r="D21" s="19" t="s">
+        <v>354</v>
+      </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -3070,10 +3095,16 @@
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="16"/>
+      <c r="A22" s="24">
+        <v>45693</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>351</v>
+      </c>
       <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
+      <c r="D22" s="19" t="s">
+        <v>355</v>
+      </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3084,7 +3115,16 @@
       <c r="AL22" s="7"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A23" s="24">
+        <v>45700</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>353</v>
+      </c>
       <c r="C23" s="17"/>
+      <c r="D23" s="19" t="s">
+        <v>356</v>
+      </c>
       <c r="M23" s="3" t="s">
         <v>33</v>
       </c>
@@ -3106,6 +3146,12 @@
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A24" s="24">
+        <v>45707</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>351</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="M24" s="3" t="s">
         <v>33</v>
@@ -3127,122 +3173,182 @@
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A25" s="24">
+        <v>45714</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>353</v>
+      </c>
       <c r="M25" s="3" t="s">
         <v>33</v>
       </c>
       <c r="W25" s="4"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A26" s="24">
+        <v>45721</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>351</v>
+      </c>
       <c r="M26" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A27" s="24">
+        <v>45728</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>352</v>
+      </c>
       <c r="M27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A28" s="24">
+        <v>45735</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>351</v>
+      </c>
       <c r="M28" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A29" s="24">
+        <v>45742</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>353</v>
+      </c>
       <c r="M29" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A30" s="24">
+        <v>45749</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>351</v>
+      </c>
       <c r="M30" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A31" s="24">
+        <v>45756</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>353</v>
+      </c>
       <c r="M31" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.3">
+      <c r="A32" s="24">
+        <v>45763</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>351</v>
+      </c>
       <c r="M32" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" s="24">
+        <v>45770</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>353</v>
+      </c>
       <c r="M33" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A34" s="24">
+        <v>45777</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>351</v>
+      </c>
       <c r="M34" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M35" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M36" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M37" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M38" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M39" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M40" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M41" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M42" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M43" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M44" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M45" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M46" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M47" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M48" s="3" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Updates to spring 2025 workshop schedule
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49512439-A6C6-4736-973C-539D6139E3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F4E72D-916E-48D7-B595-01CAE87D7794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="360">
   <si>
     <t>Date</t>
   </si>
@@ -1115,6 +1115,9 @@
   </si>
   <si>
     <t>ling, monique, econ JMC,</t>
+  </si>
+  <si>
+    <t>Ling Yao, Monique Davis, econ JMC,</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1125,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1281,10 +1284,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1602,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D9866-1A44-4963-B386-3AED68110417}">
   <dimension ref="A1:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1641,51 +1644,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
       <c r="L1" s="1"/>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
       <c r="W1" s="1"/>
-      <c r="Y1" s="23" t="s">
+      <c r="Y1" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AD1" s="23" t="s">
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AD1" s="24" t="s">
         <v>273</v>
       </c>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AK1" s="23" t="s">
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AK1" s="24" t="s">
         <v>274</v>
       </c>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
+      <c r="AL1" s="24"/>
+      <c r="AM1" s="24"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2705,6 +2708,9 @@
         <v>311</v>
       </c>
       <c r="C15" s="11"/>
+      <c r="D15" s="12" t="s">
+        <v>357</v>
+      </c>
       <c r="G15" s="9"/>
       <c r="H15" s="8"/>
       <c r="L15" s="4"/>
@@ -2774,7 +2780,9 @@
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="19" t="s">
+        <v>354</v>
+      </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -2837,7 +2845,9 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C17" s="22"/>
-      <c r="D17" s="11"/>
+      <c r="D17" s="19" t="s">
+        <v>355</v>
+      </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -2901,7 +2911,9 @@
       <c r="A18" s="8"/>
       <c r="B18" s="16"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
+      <c r="D18" s="19" t="s">
+        <v>356</v>
+      </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -3015,16 +3027,13 @@
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A20" s="24">
+      <c r="A20" s="23">
         <v>45679</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>351</v>
       </c>
       <c r="C20" s="11"/>
-      <c r="D20" s="12" t="s">
-        <v>357</v>
-      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -3057,19 +3066,28 @@
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A21" s="24">
+      <c r="A21" s="23">
         <v>45686</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>353</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="19" t="s">
-        <v>354</v>
-      </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="C21" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="G21" t="s">
+        <v>270</v>
+      </c>
+      <c r="H21" t="s">
+        <v>306</v>
+      </c>
       <c r="M21" s="3" t="s">
         <v>33</v>
       </c>
@@ -3095,16 +3113,13 @@
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A22" s="24">
+      <c r="A22" s="23">
         <v>45693</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>351</v>
       </c>
       <c r="C22" s="11"/>
-      <c r="D22" s="19" t="s">
-        <v>355</v>
-      </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -3115,16 +3130,13 @@
       <c r="AL22" s="7"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A23" s="24">
+      <c r="A23" s="23">
         <v>45700</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>353</v>
       </c>
       <c r="C23" s="17"/>
-      <c r="D23" s="19" t="s">
-        <v>356</v>
-      </c>
       <c r="M23" s="3" t="s">
         <v>33</v>
       </c>
@@ -3146,7 +3158,7 @@
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A24" s="24">
+      <c r="A24" s="23">
         <v>45707</v>
       </c>
       <c r="B24" s="16" t="s">
@@ -3173,7 +3185,7 @@
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A25" s="24">
+      <c r="A25" s="23">
         <v>45714</v>
       </c>
       <c r="B25" s="16" t="s">
@@ -3185,7 +3197,7 @@
       <c r="W25" s="4"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A26" s="24">
+      <c r="A26" s="23">
         <v>45721</v>
       </c>
       <c r="B26" s="13" t="s">
@@ -3196,7 +3208,7 @@
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A27" s="24">
+      <c r="A27" s="23">
         <v>45728</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -3207,7 +3219,7 @@
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A28" s="24">
+      <c r="A28" s="23">
         <v>45735</v>
       </c>
       <c r="B28" s="16" t="s">
@@ -3218,18 +3230,34 @@
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A29" s="24">
+      <c r="A29" s="23">
         <v>45742</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>353</v>
       </c>
+      <c r="C29" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="G29" t="s">
+        <v>269</v>
+      </c>
+      <c r="H29" t="s">
+        <v>268</v>
+      </c>
       <c r="M29" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A30" s="24">
+      <c r="A30" s="23">
         <v>45749</v>
       </c>
       <c r="B30" s="16" t="s">
@@ -3240,7 +3268,7 @@
       </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A31" s="24">
+      <c r="A31" s="23">
         <v>45756</v>
       </c>
       <c r="B31" s="16" t="s">
@@ -3251,7 +3279,7 @@
       </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A32" s="24">
+      <c r="A32" s="23">
         <v>45763</v>
       </c>
       <c r="B32" s="16" t="s">
@@ -3262,18 +3290,34 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="24">
+      <c r="A33" s="23">
         <v>45770</v>
       </c>
       <c r="B33" s="16" t="s">
         <v>353</v>
       </c>
+      <c r="C33" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>284</v>
+      </c>
       <c r="M33" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="24">
+      <c r="A34" s="23">
         <v>45777</v>
       </c>
       <c r="B34" s="13" t="s">

</xml_diff>

<commit_message>
Update attendance for Natalia presentation
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F4E72D-916E-48D7-B595-01CAE87D7794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABA2C6D-0A0A-4712-B223-9E458E984734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Presentations" sheetId="1" r:id="rId1"/>
@@ -1117,7 +1117,7 @@
     <t>ling, monique, econ JMC,</t>
   </si>
   <si>
-    <t>Ling Yao, Monique Davis, econ JMC,</t>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -1605,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D9866-1A44-4963-B386-3AED68110417}">
   <dimension ref="A1:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Natalia workshop video'
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanm\Documents\apecseminar.github.io\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABA2C6D-0A0A-4712-B223-9E458E984734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8805595-A787-4CF8-B073-CD2905136373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Current Presentations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="361">
   <si>
     <t>Date</t>
   </si>
@@ -1118,6 +1118,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Teaching as a Graduate Student</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1266,9 +1269,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1605,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D9866-1A44-4963-B386-3AED68110417}">
   <dimension ref="A1:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1644,51 +1644,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
       <c r="L1" s="1"/>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="24"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
       <c r="W1" s="1"/>
-      <c r="Y1" s="24" t="s">
+      <c r="Y1" s="23" t="s">
         <v>194</v>
       </c>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="24"/>
-      <c r="AD1" s="24" t="s">
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AD1" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AK1" s="24" t="s">
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AK1" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1739,7 +1739,7 @@
       <c r="Q2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="R2" s="17" t="s">
         <v>3</v>
       </c>
       <c r="S2" s="2" t="s">
@@ -2556,7 +2556,7 @@
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="D12" s="21"/>
+      <c r="D12" s="20"/>
       <c r="L12" s="4"/>
       <c r="M12" s="3" t="s">
         <v>33</v>
@@ -2607,8 +2607,8 @@
       <c r="A13" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
       <c r="I13" s="9"/>
       <c r="L13" s="4"/>
       <c r="M13" s="3" t="s">
@@ -2674,7 +2674,7 @@
       <c r="O14" s="16"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="8"/>
-      <c r="R14" s="20"/>
+      <c r="R14" s="19"/>
       <c r="S14" s="9"/>
       <c r="W14" s="4"/>
       <c r="X14" s="3" t="s">
@@ -2727,7 +2727,7 @@
         <v>15</v>
       </c>
       <c r="Q15" s="8"/>
-      <c r="R15" s="19" t="s">
+      <c r="R15" s="18" t="s">
         <v>169</v>
       </c>
       <c r="S15" t="s">
@@ -2780,7 +2780,7 @@
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="C16" s="11"/>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>354</v>
       </c>
       <c r="E16" s="9"/>
@@ -2844,8 +2844,8 @@
       </c>
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="C17" s="22"/>
-      <c r="D17" s="19" t="s">
+      <c r="C17" s="21"/>
+      <c r="D17" s="18" t="s">
         <v>355</v>
       </c>
       <c r="E17" s="9"/>
@@ -2866,7 +2866,7 @@
         <v>358</v>
       </c>
       <c r="Q17" s="8"/>
-      <c r="R17" s="19" t="s">
+      <c r="R17" s="18" t="s">
         <v>38</v>
       </c>
       <c r="S17" s="8" t="s">
@@ -2911,7 +2911,7 @@
       <c r="A18" s="8"/>
       <c r="B18" s="16"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>356</v>
       </c>
       <c r="E18" s="9"/>
@@ -2931,7 +2931,7 @@
         <v>15</v>
       </c>
       <c r="Q18" s="8"/>
-      <c r="R18" s="19" t="s">
+      <c r="R18" s="18" t="s">
         <v>169</v>
       </c>
       <c r="S18" t="s">
@@ -2992,7 +2992,7 @@
       <c r="O19"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="8"/>
-      <c r="R19" s="20"/>
+      <c r="R19" s="19"/>
       <c r="S19" s="9"/>
       <c r="W19" s="4"/>
       <c r="X19" s="3" t="s">
@@ -3027,7 +3027,7 @@
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
+      <c r="A20" s="22">
         <v>45679</v>
       </c>
       <c r="B20" s="16" t="s">
@@ -3046,7 +3046,7 @@
       <c r="O20" s="16"/>
       <c r="P20" s="11"/>
       <c r="Q20" s="8"/>
-      <c r="R20" s="20"/>
+      <c r="R20" s="19"/>
       <c r="S20" s="9"/>
       <c r="W20" s="4"/>
       <c r="X20" s="3" t="s">
@@ -3066,7 +3066,7 @@
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A21" s="23">
+      <c r="A21" s="22">
         <v>45686</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -3079,7 +3079,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="18" t="s">
         <v>169</v>
       </c>
       <c r="G21" t="s">
@@ -3113,7 +3113,7 @@
       </c>
     </row>
     <row r="22" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A22" s="23">
+      <c r="A22" s="22">
         <v>45693</v>
       </c>
       <c r="B22" s="16" t="s">
@@ -3130,13 +3130,27 @@
       <c r="AL22" s="7"/>
     </row>
     <row r="23" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A23" s="23">
+      <c r="A23" s="22">
         <v>45700</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>353</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" t="s">
+        <v>272</v>
+      </c>
+      <c r="H23" t="s">
+        <v>360</v>
+      </c>
       <c r="M23" s="3" t="s">
         <v>33</v>
       </c>
@@ -3158,7 +3172,7 @@
       </c>
     </row>
     <row r="24" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A24" s="23">
+      <c r="A24" s="22">
         <v>45707</v>
       </c>
       <c r="B24" s="16" t="s">
@@ -3185,7 +3199,7 @@
       </c>
     </row>
     <row r="25" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A25" s="23">
+      <c r="A25" s="22">
         <v>45714</v>
       </c>
       <c r="B25" s="16" t="s">
@@ -3197,7 +3211,7 @@
       <c r="W25" s="4"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A26" s="23">
+      <c r="A26" s="22">
         <v>45721</v>
       </c>
       <c r="B26" s="13" t="s">
@@ -3208,7 +3222,7 @@
       </c>
     </row>
     <row r="27" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A27" s="23">
+      <c r="A27" s="22">
         <v>45728</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -3219,7 +3233,7 @@
       </c>
     </row>
     <row r="28" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A28" s="23">
+      <c r="A28" s="22">
         <v>45735</v>
       </c>
       <c r="B28" s="16" t="s">
@@ -3230,7 +3244,7 @@
       </c>
     </row>
     <row r="29" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A29" s="23">
+      <c r="A29" s="22">
         <v>45742</v>
       </c>
       <c r="B29" s="16" t="s">
@@ -3243,7 +3257,7 @@
         <v>15</v>
       </c>
       <c r="E29" s="8"/>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="18" t="s">
         <v>169</v>
       </c>
       <c r="G29" t="s">
@@ -3257,7 +3271,7 @@
       </c>
     </row>
     <row r="30" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A30" s="23">
+      <c r="A30" s="22">
         <v>45749</v>
       </c>
       <c r="B30" s="16" t="s">
@@ -3268,18 +3282,33 @@
       </c>
     </row>
     <row r="31" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A31" s="23">
+      <c r="A31" s="22">
         <v>45756</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>353</v>
       </c>
+      <c r="C31" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" t="s">
+        <v>270</v>
+      </c>
+      <c r="H31" t="s">
+        <v>259</v>
+      </c>
       <c r="M31" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="A32" s="23">
+      <c r="A32" s="22">
         <v>45763</v>
       </c>
       <c r="B32" s="16" t="s">
@@ -3290,7 +3319,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="23">
+      <c r="A33" s="22">
         <v>45770</v>
       </c>
       <c r="B33" s="16" t="s">
@@ -3303,7 +3332,7 @@
         <v>359</v>
       </c>
       <c r="E33" s="8"/>
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="18" t="s">
         <v>38</v>
       </c>
       <c r="G33" s="8" t="s">
@@ -3317,7 +3346,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="23">
+      <c r="A34" s="22">
         <v>45777</v>
       </c>
       <c r="B34" s="13" t="s">

</xml_diff>

<commit_message>
Updated attendnace for Ana Melissa presentation
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8805595-A787-4CF8-B073-CD2905136373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C003D48-14CB-4DF1-98E9-60C5D3DD678C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="363">
   <si>
     <t>Date</t>
   </si>
@@ -1121,6 +1121,12 @@
   </si>
   <si>
     <t>Teaching as a Graduate Student</t>
+  </si>
+  <si>
+    <t>Doubly Robust Estimators and Covariate Selection</t>
+  </si>
+  <si>
+    <t>Ryan (Pollination)</t>
   </si>
 </sst>
 </file>
@@ -1605,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D9866-1A44-4963-B386-3AED68110417}">
   <dimension ref="A1:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2779,6 +2785,9 @@
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>362</v>
+      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="18" t="s">
         <v>354</v>
@@ -3301,7 +3310,7 @@
         <v>270</v>
       </c>
       <c r="H31" t="s">
-        <v>259</v>
+        <v>361</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Moved schedule to past schedules. Updated website.
</commit_message>
<xml_diff>
--- a/notes/scheduling.xlsx
+++ b/notes/scheduling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apecseminar.github.io\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C003D48-14CB-4DF1-98E9-60C5D3DD678C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34EA6FC-DE29-41C8-81A6-CA5A513FED05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3A95A67A-AA40-466E-A02C-B6088C2210BE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="362">
   <si>
     <t>Date</t>
   </si>
@@ -1102,15 +1102,6 @@
     <t>workshop</t>
   </si>
   <si>
-    <t>Schedule the 4 speaker slots, and then remove remaining workshops</t>
-  </si>
-  <si>
-    <t>Send call for presenters, all options, then select a couple for free discussions</t>
-  </si>
-  <si>
-    <t>Then settle on schedule and annonce</t>
-  </si>
-  <si>
     <t>Wednesdays from 11 AM - 12 PM</t>
   </si>
   <si>
@@ -1127,6 +1118,12 @@
   </si>
   <si>
     <t>Ryan (Pollination)</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Carmen</t>
   </si>
 </sst>
 </file>
@@ -1611,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946D9866-1A44-4963-B386-3AED68110417}">
   <dimension ref="A1:AR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2715,7 +2712,7 @@
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="12" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="8"/>
@@ -2786,12 +2783,10 @@
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B16" s="13" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="18" t="s">
-        <v>354</v>
-      </c>
+      <c r="D16" s="18"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -2854,9 +2849,7 @@
     </row>
     <row r="17" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C17" s="21"/>
-      <c r="D17" s="18" t="s">
-        <v>355</v>
-      </c>
+      <c r="D17" s="18"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -2872,7 +2865,7 @@
         <v>283</v>
       </c>
       <c r="P17" s="11" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="Q17" s="8"/>
       <c r="R17" s="18" t="s">
@@ -2920,9 +2913,7 @@
       <c r="A18" s="8"/>
       <c r="B18" s="16"/>
       <c r="C18" s="11"/>
-      <c r="D18" s="18" t="s">
-        <v>356</v>
-      </c>
+      <c r="D18" s="18"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -3097,6 +3088,9 @@
       <c r="H21" t="s">
         <v>306</v>
       </c>
+      <c r="I21" t="s">
+        <v>360</v>
+      </c>
       <c r="M21" s="3" t="s">
         <v>33</v>
       </c>
@@ -3158,7 +3152,10 @@
         <v>272</v>
       </c>
       <c r="H23" t="s">
-        <v>360</v>
+        <v>357</v>
+      </c>
+      <c r="I23" t="s">
+        <v>361</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>33</v>
@@ -3275,6 +3272,9 @@
       <c r="H29" t="s">
         <v>268</v>
       </c>
+      <c r="I29" t="s">
+        <v>360</v>
+      </c>
       <c r="M29" s="3" t="s">
         <v>33</v>
       </c>
@@ -3310,6 +3310,9 @@
         <v>270</v>
       </c>
       <c r="H31" t="s">
+        <v>358</v>
+      </c>
+      <c r="I31" t="s">
         <v>361</v>
       </c>
       <c r="M31" s="3" t="s">
@@ -3338,7 +3341,7 @@
         <v>283</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="18" t="s">
@@ -3349,6 +3352,9 @@
       </c>
       <c r="H33" s="8" t="s">
         <v>284</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>360</v>
       </c>
       <c r="M33" s="3" t="s">
         <v>33</v>

</xml_diff>